<commit_message>
atualização de tabela e modelo
</commit_message>
<xml_diff>
--- a/Torque-RPM lookuptable.xlsx
+++ b/Torque-RPM lookuptable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\OneDrive\Documentos\GitHub\ufpe-project-bsg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7706ECB-77F1-498D-B3EF-74ACA83F0C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D2C33E3-AC88-4EDA-86D5-A2AF8FF9EB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D9DA52EB-1665-42CA-8574-C6888C21CC1B}"/>
   </bookViews>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219CBD8E-9D27-420D-9A84-EAFCE9AEDC37}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H187" sqref="H187"/>
+    <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
+      <selection activeCell="I197" sqref="I197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -439,7 +439,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="2">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -447,7 +447,7 @@
         <v>100</v>
       </c>
       <c r="B3" s="2">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -455,7 +455,7 @@
         <v>150</v>
       </c>
       <c r="B4" s="2">
-        <v>60</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -463,7 +463,7 @@
         <v>200</v>
       </c>
       <c r="B5" s="2">
-        <v>80</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -471,7 +471,7 @@
         <v>250</v>
       </c>
       <c r="B6" s="2">
-        <v>100</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -479,7 +479,7 @@
         <v>300</v>
       </c>
       <c r="B7" s="2">
-        <v>120</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -487,7 +487,7 @@
         <v>350</v>
       </c>
       <c r="B8" s="2">
-        <v>140</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -495,7 +495,7 @@
         <v>400</v>
       </c>
       <c r="B9" s="2">
-        <v>160</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -503,7 +503,7 @@
         <v>450</v>
       </c>
       <c r="B10" s="2">
-        <v>180</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -511,7 +511,7 @@
         <v>500</v>
       </c>
       <c r="B11" s="2">
-        <v>200</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -519,7 +519,7 @@
         <v>550</v>
       </c>
       <c r="B12" s="2">
-        <v>220</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -527,7 +527,7 @@
         <v>600</v>
       </c>
       <c r="B13" s="2">
-        <v>240</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -535,7 +535,7 @@
         <v>650</v>
       </c>
       <c r="B14" s="2">
-        <v>260</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -543,7 +543,7 @@
         <v>700</v>
       </c>
       <c r="B15" s="2">
-        <v>280</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -551,7 +551,7 @@
         <v>750</v>
       </c>
       <c r="B16" s="2">
-        <v>300</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -559,7 +559,7 @@
         <v>800</v>
       </c>
       <c r="B17" s="2">
-        <v>320</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -567,7 +567,7 @@
         <v>850</v>
       </c>
       <c r="B18" s="2">
-        <v>340</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -575,7 +575,7 @@
         <v>900</v>
       </c>
       <c r="B19" s="2">
-        <v>360</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -583,7 +583,7 @@
         <v>950</v>
       </c>
       <c r="B20" s="2">
-        <v>380</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -591,7 +591,7 @@
         <v>1000</v>
       </c>
       <c r="B21" s="2">
-        <v>400</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -599,7 +599,7 @@
         <v>1050</v>
       </c>
       <c r="B22" s="2">
-        <v>420</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -607,7 +607,7 @@
         <v>1100</v>
       </c>
       <c r="B23" s="2">
-        <v>440</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -615,7 +615,7 @@
         <v>1150</v>
       </c>
       <c r="B24" s="2">
-        <v>460</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -623,7 +623,7 @@
         <v>1200</v>
       </c>
       <c r="B25" s="2">
-        <v>480</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -631,7 +631,7 @@
         <v>1250</v>
       </c>
       <c r="B26" s="2">
-        <v>500</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -639,7 +639,7 @@
         <v>1300</v>
       </c>
       <c r="B27" s="2">
-        <v>520</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -647,7 +647,7 @@
         <v>1350</v>
       </c>
       <c r="B28" s="2">
-        <v>540</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -655,7 +655,7 @@
         <v>1400</v>
       </c>
       <c r="B29" s="2">
-        <v>560</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -663,7 +663,7 @@
         <v>1450</v>
       </c>
       <c r="B30" s="2">
-        <v>580</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -671,7 +671,7 @@
         <v>1500</v>
       </c>
       <c r="B31" s="2">
-        <v>600</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -679,7 +679,7 @@
         <v>1550</v>
       </c>
       <c r="B32" s="2">
-        <v>620</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -687,7 +687,7 @@
         <v>1600</v>
       </c>
       <c r="B33" s="2">
-        <v>640</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -695,7 +695,7 @@
         <v>1650</v>
       </c>
       <c r="B34" s="2">
-        <v>660</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -703,7 +703,7 @@
         <v>1700</v>
       </c>
       <c r="B35" s="2">
-        <v>680</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,7 +711,7 @@
         <v>1750</v>
       </c>
       <c r="B36" s="2">
-        <v>700</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -719,7 +719,7 @@
         <v>1800</v>
       </c>
       <c r="B37" s="2">
-        <v>720</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -727,7 +727,7 @@
         <v>1850</v>
       </c>
       <c r="B38" s="2">
-        <v>740</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -735,7 +735,7 @@
         <v>1900</v>
       </c>
       <c r="B39" s="2">
-        <v>760</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -743,7 +743,7 @@
         <v>1950</v>
       </c>
       <c r="B40" s="2">
-        <v>780</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -751,7 +751,7 @@
         <v>2000</v>
       </c>
       <c r="B41" s="2">
-        <v>800</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -759,7 +759,7 @@
         <v>2050</v>
       </c>
       <c r="B42" s="2">
-        <v>820</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -767,7 +767,7 @@
         <v>2100</v>
       </c>
       <c r="B43" s="2">
-        <v>840</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -775,7 +775,7 @@
         <v>2150</v>
       </c>
       <c r="B44" s="2">
-        <v>860</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -783,7 +783,7 @@
         <v>2200</v>
       </c>
       <c r="B45" s="2">
-        <v>880</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -791,7 +791,7 @@
         <v>2250</v>
       </c>
       <c r="B46" s="2">
-        <v>900</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -799,7 +799,7 @@
         <v>2300</v>
       </c>
       <c r="B47" s="2">
-        <v>920</v>
+        <v>93</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -807,7 +807,7 @@
         <v>2350</v>
       </c>
       <c r="B48" s="2">
-        <v>940</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -815,7 +815,7 @@
         <v>2400</v>
       </c>
       <c r="B49" s="2">
-        <v>960</v>
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -823,7 +823,7 @@
         <v>2450</v>
       </c>
       <c r="B50" s="2">
-        <v>980</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -831,7 +831,7 @@
         <v>2500</v>
       </c>
       <c r="B51" s="2">
-        <v>1000</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -839,7 +839,7 @@
         <v>2550</v>
       </c>
       <c r="B52" s="2">
-        <v>1020</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -847,7 +847,7 @@
         <v>2600</v>
       </c>
       <c r="B53" s="2">
-        <v>1040</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -855,7 +855,7 @@
         <v>2650</v>
       </c>
       <c r="B54" s="2">
-        <v>1060</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -863,7 +863,7 @@
         <v>2700</v>
       </c>
       <c r="B55" s="2">
-        <v>1080</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -871,7 +871,7 @@
         <v>2750</v>
       </c>
       <c r="B56" s="2">
-        <v>1100</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -879,7 +879,7 @@
         <v>2800</v>
       </c>
       <c r="B57" s="2">
-        <v>1120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -887,7 +887,7 @@
         <v>2850</v>
       </c>
       <c r="B58" s="2">
-        <v>1140</v>
+        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -895,7 +895,7 @@
         <v>2900</v>
       </c>
       <c r="B59" s="2">
-        <v>1160</v>
+        <v>117</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -903,7 +903,7 @@
         <v>2950</v>
       </c>
       <c r="B60" s="2">
-        <v>1180</v>
+        <v>119</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -911,7 +911,7 @@
         <v>3000</v>
       </c>
       <c r="B61" s="2">
-        <v>1200</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -919,7 +919,7 @@
         <v>3050</v>
       </c>
       <c r="B62" s="2">
-        <v>1220</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -927,7 +927,7 @@
         <v>3100</v>
       </c>
       <c r="B63" s="2">
-        <v>1240</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -935,7 +935,7 @@
         <v>3150</v>
       </c>
       <c r="B64" s="2">
-        <v>1260</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -943,7 +943,7 @@
         <v>3200</v>
       </c>
       <c r="B65" s="2">
-        <v>1280</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -951,7 +951,7 @@
         <v>3250</v>
       </c>
       <c r="B66" s="2">
-        <v>1300</v>
+        <v>131</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -959,7 +959,7 @@
         <v>3300</v>
       </c>
       <c r="B67" s="2">
-        <v>1320</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -967,7 +967,7 @@
         <v>3350</v>
       </c>
       <c r="B68" s="2">
-        <v>1340</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -975,7 +975,7 @@
         <v>3400</v>
       </c>
       <c r="B69" s="2">
-        <v>1360</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -983,7 +983,7 @@
         <v>3450</v>
       </c>
       <c r="B70" s="2">
-        <v>1380</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -991,7 +991,7 @@
         <v>3500</v>
       </c>
       <c r="B71" s="2">
-        <v>1400</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -999,7 +999,7 @@
         <v>3550</v>
       </c>
       <c r="B72" s="2">
-        <v>1420</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -1007,7 +1007,7 @@
         <v>3600</v>
       </c>
       <c r="B73" s="2">
-        <v>1440</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1015,7 +1015,7 @@
         <v>3650</v>
       </c>
       <c r="B74" s="2">
-        <v>1460</v>
+        <v>147</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1023,7 +1023,7 @@
         <v>3700</v>
       </c>
       <c r="B75" s="2">
-        <v>1480</v>
+        <v>149</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1031,7 +1031,7 @@
         <v>3750</v>
       </c>
       <c r="B76" s="2">
-        <v>1500</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1039,7 +1039,7 @@
         <v>3800</v>
       </c>
       <c r="B77" s="2">
-        <v>1520</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1047,7 +1047,7 @@
         <v>3850</v>
       </c>
       <c r="B78" s="2">
-        <v>1540</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1055,7 +1055,7 @@
         <v>3900</v>
       </c>
       <c r="B79" s="2">
-        <v>1560</v>
+        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1063,7 +1063,7 @@
         <v>3950</v>
       </c>
       <c r="B80" s="2">
-        <v>1580</v>
+        <v>159</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1071,7 +1071,7 @@
         <v>4000</v>
       </c>
       <c r="B81" s="2">
-        <v>1600</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1079,7 +1079,7 @@
         <v>4050</v>
       </c>
       <c r="B82" s="2">
-        <v>1620</v>
+        <v>163</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1087,7 +1087,7 @@
         <v>4100</v>
       </c>
       <c r="B83" s="2">
-        <v>1640</v>
+        <v>165</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1095,7 +1095,7 @@
         <v>4150</v>
       </c>
       <c r="B84" s="2">
-        <v>1660</v>
+        <v>167</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1103,7 +1103,7 @@
         <v>4200</v>
       </c>
       <c r="B85" s="2">
-        <v>1680</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1111,7 +1111,7 @@
         <v>4250</v>
       </c>
       <c r="B86" s="2">
-        <v>1700</v>
+        <v>171</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1119,7 +1119,7 @@
         <v>4300</v>
       </c>
       <c r="B87" s="2">
-        <v>1720</v>
+        <v>173</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -1127,7 +1127,7 @@
         <v>4350</v>
       </c>
       <c r="B88" s="2">
-        <v>1740</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -1135,7 +1135,7 @@
         <v>4400</v>
       </c>
       <c r="B89" s="2">
-        <v>1760</v>
+        <v>177</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -1143,7 +1143,7 @@
         <v>4450</v>
       </c>
       <c r="B90" s="2">
-        <v>1780</v>
+        <v>179</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -1151,7 +1151,7 @@
         <v>4500</v>
       </c>
       <c r="B91" s="2">
-        <v>1800</v>
+        <v>181</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1159,7 +1159,7 @@
         <v>4550</v>
       </c>
       <c r="B92" s="2">
-        <v>1820</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1167,7 +1167,7 @@
         <v>4600</v>
       </c>
       <c r="B93" s="2">
-        <v>1840</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -1175,7 +1175,7 @@
         <v>4650</v>
       </c>
       <c r="B94" s="2">
-        <v>1860</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1183,7 +1183,7 @@
         <v>4700</v>
       </c>
       <c r="B95" s="2">
-        <v>1880</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1191,7 +1191,7 @@
         <v>4750</v>
       </c>
       <c r="B96" s="2">
-        <v>1900</v>
+        <v>191</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -1199,7 +1199,7 @@
         <v>4800</v>
       </c>
       <c r="B97" s="2">
-        <v>1920</v>
+        <v>193</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -1207,7 +1207,7 @@
         <v>4850</v>
       </c>
       <c r="B98" s="2">
-        <v>1940</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -1215,7 +1215,7 @@
         <v>4900</v>
       </c>
       <c r="B99" s="2">
-        <v>1960</v>
+        <v>197</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -1223,7 +1223,7 @@
         <v>4950</v>
       </c>
       <c r="B100" s="2">
-        <v>1980</v>
+        <v>199</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -1231,7 +1231,7 @@
         <v>5000</v>
       </c>
       <c r="B101" s="2">
-        <v>2000</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -1239,7 +1239,7 @@
         <v>5050</v>
       </c>
       <c r="B102" s="2">
-        <v>2020</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -1247,7 +1247,7 @@
         <v>5100</v>
       </c>
       <c r="B103" s="2">
-        <v>2040</v>
+        <v>205</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -1255,7 +1255,7 @@
         <v>5150</v>
       </c>
       <c r="B104" s="2">
-        <v>2060</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -1263,7 +1263,7 @@
         <v>5200</v>
       </c>
       <c r="B105" s="2">
-        <v>2080</v>
+        <v>209</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -1271,7 +1271,7 @@
         <v>5250</v>
       </c>
       <c r="B106" s="2">
-        <v>2100</v>
+        <v>211</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -1279,7 +1279,7 @@
         <v>5300</v>
       </c>
       <c r="B107" s="2">
-        <v>2120</v>
+        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -1287,7 +1287,7 @@
         <v>5350</v>
       </c>
       <c r="B108" s="2">
-        <v>2140</v>
+        <v>215</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -1295,7 +1295,7 @@
         <v>5400</v>
       </c>
       <c r="B109" s="2">
-        <v>2160</v>
+        <v>217</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -1303,7 +1303,7 @@
         <v>5450</v>
       </c>
       <c r="B110" s="2">
-        <v>2180</v>
+        <v>219</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -1311,7 +1311,7 @@
         <v>5500</v>
       </c>
       <c r="B111" s="2">
-        <v>2200</v>
+        <v>221</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -1319,7 +1319,7 @@
         <v>5550</v>
       </c>
       <c r="B112" s="2">
-        <v>2220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -1327,7 +1327,7 @@
         <v>5600</v>
       </c>
       <c r="B113" s="2">
-        <v>2240</v>
+        <v>225</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -1335,7 +1335,7 @@
         <v>5650</v>
       </c>
       <c r="B114" s="2">
-        <v>2260</v>
+        <v>227</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -1343,7 +1343,7 @@
         <v>5700</v>
       </c>
       <c r="B115" s="2">
-        <v>2280</v>
+        <v>229</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -1351,7 +1351,7 @@
         <v>5750</v>
       </c>
       <c r="B116" s="2">
-        <v>2300</v>
+        <v>231</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -1359,7 +1359,7 @@
         <v>5800</v>
       </c>
       <c r="B117" s="2">
-        <v>2320</v>
+        <v>233</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -1367,7 +1367,7 @@
         <v>5850</v>
       </c>
       <c r="B118" s="2">
-        <v>2340</v>
+        <v>235</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -1375,7 +1375,7 @@
         <v>5900</v>
       </c>
       <c r="B119" s="2">
-        <v>2360</v>
+        <v>237</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
@@ -1383,7 +1383,7 @@
         <v>5950</v>
       </c>
       <c r="B120" s="2">
-        <v>2380</v>
+        <v>239</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
@@ -1391,7 +1391,7 @@
         <v>6000</v>
       </c>
       <c r="B121" s="2">
-        <v>2400</v>
+        <v>241</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
@@ -1399,7 +1399,7 @@
         <v>6050</v>
       </c>
       <c r="B122" s="2">
-        <v>2420</v>
+        <v>243</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
@@ -1407,7 +1407,7 @@
         <v>6100</v>
       </c>
       <c r="B123" s="2">
-        <v>2440</v>
+        <v>245</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
@@ -1415,7 +1415,7 @@
         <v>6150</v>
       </c>
       <c r="B124" s="2">
-        <v>2460</v>
+        <v>247</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
@@ -1423,7 +1423,7 @@
         <v>6200</v>
       </c>
       <c r="B125" s="2">
-        <v>2480</v>
+        <v>249</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -1431,7 +1431,7 @@
         <v>6250</v>
       </c>
       <c r="B126" s="2">
-        <v>2500</v>
+        <v>251</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
@@ -1439,7 +1439,7 @@
         <v>6300</v>
       </c>
       <c r="B127" s="2">
-        <v>2520</v>
+        <v>253</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -1447,7 +1447,7 @@
         <v>6350</v>
       </c>
       <c r="B128" s="2">
-        <v>2540</v>
+        <v>255</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -1455,7 +1455,7 @@
         <v>6400</v>
       </c>
       <c r="B129" s="2">
-        <v>2560</v>
+        <v>257</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
@@ -1463,7 +1463,7 @@
         <v>6450</v>
       </c>
       <c r="B130" s="2">
-        <v>2580</v>
+        <v>259</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
@@ -1471,7 +1471,7 @@
         <v>6500</v>
       </c>
       <c r="B131" s="2">
-        <v>2600</v>
+        <v>261</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
@@ -1479,7 +1479,7 @@
         <v>6550</v>
       </c>
       <c r="B132" s="2">
-        <v>2580</v>
+        <v>259</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
@@ -1487,7 +1487,7 @@
         <v>6600</v>
       </c>
       <c r="B133" s="2">
-        <v>2560</v>
+        <v>257</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
@@ -1495,7 +1495,7 @@
         <v>6650</v>
       </c>
       <c r="B134" s="2">
-        <v>2540</v>
+        <v>255</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
@@ -1503,7 +1503,7 @@
         <v>6700</v>
       </c>
       <c r="B135" s="2">
-        <v>2520</v>
+        <v>253</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
@@ -1511,7 +1511,7 @@
         <v>6750</v>
       </c>
       <c r="B136" s="2">
-        <v>2500</v>
+        <v>251</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -1519,7 +1519,7 @@
         <v>6800</v>
       </c>
       <c r="B137" s="2">
-        <v>2480</v>
+        <v>249</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
@@ -1527,7 +1527,7 @@
         <v>6850</v>
       </c>
       <c r="B138" s="2">
-        <v>2460</v>
+        <v>247</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
@@ -1535,7 +1535,7 @@
         <v>6900</v>
       </c>
       <c r="B139" s="2">
-        <v>2440</v>
+        <v>245</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
@@ -1543,7 +1543,7 @@
         <v>6950</v>
       </c>
       <c r="B140" s="2">
-        <v>2420</v>
+        <v>243</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
@@ -1551,7 +1551,7 @@
         <v>7000</v>
       </c>
       <c r="B141" s="2">
-        <v>2400</v>
+        <v>241</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
@@ -1559,7 +1559,7 @@
         <v>7050</v>
       </c>
       <c r="B142" s="2">
-        <v>2380</v>
+        <v>239</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
@@ -1567,7 +1567,7 @@
         <v>7100</v>
       </c>
       <c r="B143" s="2">
-        <v>2360</v>
+        <v>237</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
@@ -1575,7 +1575,7 @@
         <v>7150</v>
       </c>
       <c r="B144" s="2">
-        <v>2340</v>
+        <v>235</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
@@ -1583,7 +1583,7 @@
         <v>7200</v>
       </c>
       <c r="B145" s="2">
-        <v>2320</v>
+        <v>233</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
@@ -1591,7 +1591,7 @@
         <v>7250</v>
       </c>
       <c r="B146" s="2">
-        <v>2300</v>
+        <v>231</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
@@ -1599,7 +1599,7 @@
         <v>7300</v>
       </c>
       <c r="B147" s="2">
-        <v>2280</v>
+        <v>229</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
@@ -1607,7 +1607,7 @@
         <v>7350</v>
       </c>
       <c r="B148" s="2">
-        <v>2260</v>
+        <v>227</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
@@ -1615,7 +1615,7 @@
         <v>7400</v>
       </c>
       <c r="B149" s="2">
-        <v>2240</v>
+        <v>225</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
@@ -1623,7 +1623,7 @@
         <v>7450</v>
       </c>
       <c r="B150" s="2">
-        <v>2220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
@@ -1631,7 +1631,7 @@
         <v>7500</v>
       </c>
       <c r="B151" s="2">
-        <v>2200</v>
+        <v>221</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
@@ -1639,7 +1639,7 @@
         <v>7550</v>
       </c>
       <c r="B152" s="2">
-        <v>2180</v>
+        <v>219</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
@@ -1647,7 +1647,7 @@
         <v>7600</v>
       </c>
       <c r="B153" s="2">
-        <v>2160</v>
+        <v>217</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -1655,7 +1655,7 @@
         <v>7650</v>
       </c>
       <c r="B154" s="2">
-        <v>2140</v>
+        <v>215</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
@@ -1663,7 +1663,7 @@
         <v>7700</v>
       </c>
       <c r="B155" s="2">
-        <v>2120</v>
+        <v>213</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
@@ -1671,7 +1671,7 @@
         <v>7750</v>
       </c>
       <c r="B156" s="2">
-        <v>2100</v>
+        <v>211</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
@@ -1679,7 +1679,7 @@
         <v>7800</v>
       </c>
       <c r="B157" s="2">
-        <v>2080</v>
+        <v>209</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
@@ -1687,7 +1687,7 @@
         <v>7850</v>
       </c>
       <c r="B158" s="2">
-        <v>2060</v>
+        <v>207</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
@@ -1695,7 +1695,7 @@
         <v>7900</v>
       </c>
       <c r="B159" s="2">
-        <v>2040</v>
+        <v>205</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
@@ -1703,7 +1703,7 @@
         <v>7950</v>
       </c>
       <c r="B160" s="2">
-        <v>2020</v>
+        <v>203</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -1711,7 +1711,7 @@
         <v>8000</v>
       </c>
       <c r="B161" s="2">
-        <v>2000</v>
+        <v>201</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
@@ -1719,7 +1719,7 @@
         <v>8050</v>
       </c>
       <c r="B162" s="2">
-        <v>1980</v>
+        <v>199</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
@@ -1727,7 +1727,7 @@
         <v>8100</v>
       </c>
       <c r="B163" s="2">
-        <v>1960</v>
+        <v>197</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
@@ -1735,7 +1735,7 @@
         <v>8150</v>
       </c>
       <c r="B164" s="2">
-        <v>1940</v>
+        <v>195</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
@@ -1743,7 +1743,7 @@
         <v>8200</v>
       </c>
       <c r="B165" s="2">
-        <v>1920</v>
+        <v>193</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
@@ -1751,7 +1751,7 @@
         <v>8250</v>
       </c>
       <c r="B166" s="2">
-        <v>1900</v>
+        <v>191</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
@@ -1759,7 +1759,7 @@
         <v>8300</v>
       </c>
       <c r="B167" s="2">
-        <v>1880</v>
+        <v>189</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
@@ -1767,7 +1767,7 @@
         <v>8350</v>
       </c>
       <c r="B168" s="2">
-        <v>1860</v>
+        <v>187</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
@@ -1775,7 +1775,7 @@
         <v>8400</v>
       </c>
       <c r="B169" s="2">
-        <v>1840</v>
+        <v>185</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
@@ -1783,7 +1783,7 @@
         <v>8450</v>
       </c>
       <c r="B170" s="2">
-        <v>1820</v>
+        <v>183</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
@@ -1791,7 +1791,7 @@
         <v>8500</v>
       </c>
       <c r="B171" s="2">
-        <v>1800</v>
+        <v>181</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -1799,7 +1799,7 @@
         <v>8550</v>
       </c>
       <c r="B172" s="2">
-        <v>1780</v>
+        <v>179</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
@@ -1807,7 +1807,7 @@
         <v>8600</v>
       </c>
       <c r="B173" s="2">
-        <v>1760</v>
+        <v>177</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
@@ -1815,7 +1815,7 @@
         <v>8650</v>
       </c>
       <c r="B174" s="2">
-        <v>1740</v>
+        <v>175</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
@@ -1823,7 +1823,7 @@
         <v>8700</v>
       </c>
       <c r="B175" s="2">
-        <v>1720</v>
+        <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
@@ -1831,7 +1831,7 @@
         <v>8750</v>
       </c>
       <c r="B176" s="2">
-        <v>1700</v>
+        <v>171</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
@@ -1839,7 +1839,7 @@
         <v>8800</v>
       </c>
       <c r="B177" s="2">
-        <v>1680</v>
+        <v>169</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
@@ -1847,7 +1847,7 @@
         <v>8850</v>
       </c>
       <c r="B178" s="2">
-        <v>1660</v>
+        <v>167</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
@@ -1855,7 +1855,7 @@
         <v>8900</v>
       </c>
       <c r="B179" s="2">
-        <v>1640</v>
+        <v>165</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
@@ -1863,7 +1863,7 @@
         <v>8950</v>
       </c>
       <c r="B180" s="2">
-        <v>1620</v>
+        <v>163</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
@@ -1871,7 +1871,7 @@
         <v>9000</v>
       </c>
       <c r="B181" s="2">
-        <v>1600</v>
+        <v>161</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
@@ -1879,7 +1879,7 @@
         <v>9050</v>
       </c>
       <c r="B182" s="2">
-        <v>1580</v>
+        <v>159</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
@@ -1887,7 +1887,7 @@
         <v>9100</v>
       </c>
       <c r="B183" s="2">
-        <v>1560</v>
+        <v>157</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
@@ -1895,7 +1895,7 @@
         <v>9150</v>
       </c>
       <c r="B184" s="2">
-        <v>1540</v>
+        <v>155</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
@@ -1903,7 +1903,7 @@
         <v>9200</v>
       </c>
       <c r="B185" s="2">
-        <v>1520</v>
+        <v>153</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
@@ -1911,7 +1911,7 @@
         <v>9250</v>
       </c>
       <c r="B186" s="2">
-        <v>1500</v>
+        <v>151</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
@@ -1919,7 +1919,7 @@
         <v>9300</v>
       </c>
       <c r="B187" s="2">
-        <v>1480</v>
+        <v>149</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
@@ -1927,7 +1927,7 @@
         <v>9350</v>
       </c>
       <c r="B188" s="2">
-        <v>1460</v>
+        <v>147</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
@@ -1935,7 +1935,7 @@
         <v>9400</v>
       </c>
       <c r="B189" s="2">
-        <v>1440</v>
+        <v>145</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
@@ -1943,7 +1943,7 @@
         <v>9450</v>
       </c>
       <c r="B190" s="2">
-        <v>1420</v>
+        <v>143</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
@@ -1951,7 +1951,7 @@
         <v>9500</v>
       </c>
       <c r="B191" s="2">
-        <v>1400</v>
+        <v>141</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
@@ -1959,7 +1959,7 @@
         <v>9550</v>
       </c>
       <c r="B192" s="2">
-        <v>1380</v>
+        <v>139</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
@@ -1967,7 +1967,7 @@
         <v>9600</v>
       </c>
       <c r="B193" s="2">
-        <v>1360</v>
+        <v>137</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
@@ -1975,7 +1975,7 @@
         <v>9650</v>
       </c>
       <c r="B194" s="2">
-        <v>1340</v>
+        <v>135</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
@@ -1983,7 +1983,7 @@
         <v>9700</v>
       </c>
       <c r="B195" s="2">
-        <v>1320</v>
+        <v>133</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
@@ -1991,7 +1991,7 @@
         <v>9750</v>
       </c>
       <c r="B196" s="2">
-        <v>1300</v>
+        <v>131</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
@@ -1999,7 +1999,7 @@
         <v>9800</v>
       </c>
       <c r="B197" s="2">
-        <v>1280</v>
+        <v>129</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
@@ -2007,7 +2007,7 @@
         <v>9850</v>
       </c>
       <c r="B198" s="2">
-        <v>1260</v>
+        <v>127</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
@@ -2015,7 +2015,7 @@
         <v>9900</v>
       </c>
       <c r="B199" s="2">
-        <v>1240</v>
+        <v>125</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
@@ -2023,7 +2023,7 @@
         <v>9950</v>
       </c>
       <c r="B200" s="2">
-        <v>1220</v>
+        <v>123</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
@@ -2031,7 +2031,7 @@
         <v>10000</v>
       </c>
       <c r="B201" s="2">
-        <v>1200</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>